<commit_message>
MH-59 BMS Current Sense Rev 2.0
- Change R2 from 120 ohms to 1 kohms
- Change C10 from 10 nF to 100 nF
- Change SPI and GND testpoints to through hole so they don't fall off
- Remove thermal relief from shunt resistor through holes and U.FL connector ground pads
- Regenerate the output files
</commit_message>
<xml_diff>
--- a/MSXIV_BMS_Current_Sense/Project Outputs for BMS_Current_Sense/BMS_Current_Sense_2.0/BMS_Current_Sense_2.0.xlsx
+++ b/MSXIV_BMS_Current_Sense/Project Outputs for BMS_Current_Sense/BMS_Current_Sense_2.0/BMS_Current_Sense_2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhawk\Documents\Midnight Sun\hardware\MSXIV_BMS_Current_Sense\Project Outputs for BMS_Current_Sense\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8AEE134-761B-43FC-9173-F48E27C2DC07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E85F2B9F-4A67-46E3-9703-F8090811BF4F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
     <t>Liam Hawkins</t>
   </si>
   <si>
-    <t>2020-03-01 4:30 PM</t>
+    <t>2020-03-16 8:06 PM</t>
   </si>
   <si>
     <t>1</t>
@@ -166,7 +166,7 @@
     <t>RES SHUNT 100UOHM 5% 36W 60MM</t>
   </si>
   <si>
-    <t>RES 120 OHM 1% 1/10W 0603</t>
+    <t>RES 1K OHM 5% 1/10W 0603</t>
   </si>
   <si>
     <t>RES 4.7K OHM 1% 1/10W 0603</t>
@@ -454,7 +454,7 @@
     <t>WSBM8518L1000JK</t>
   </si>
   <si>
-    <t>RC0603FR-07120RL</t>
+    <t>RC0603JR-071KL</t>
   </si>
   <si>
     <t>RC0603FR-074K7L</t>
@@ -547,7 +547,7 @@
     <t>541-1906-ND</t>
   </si>
   <si>
-    <t>311-120HRCT-ND</t>
+    <t>311-1.0KGRCT-ND</t>
   </si>
   <si>
     <t>311-4.70KHRCT-ND</t>
@@ -607,10 +607,10 @@
     <t>Bill of Materials for Project [BMS_Current_Sense.PrjPcb] (No PCB Document Selected)</t>
   </si>
   <si>
-    <t>4:30 PM</t>
-  </si>
-  <si>
-    <t>2020-03-01</t>
+    <t>8:06 PM</t>
+  </si>
+  <si>
+    <t>2020-03-16</t>
   </si>
   <si>
     <t>BOM_PartType</t>
@@ -1339,13 +1339,13 @@
         <v>158</v>
       </c>
       <c r="G12" s="3">
-        <v>0.59030000000000005</v>
+        <v>0.61514999999999997</v>
       </c>
       <c r="H12" s="3">
         <v>1</v>
       </c>
       <c r="I12" s="10">
-        <v>0.59030000000000005</v>
+        <v>0.61514999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1368,13 +1368,13 @@
         <v>159</v>
       </c>
       <c r="G13" s="3">
-        <v>0.25490000000000002</v>
+        <v>0.26562999999999998</v>
       </c>
       <c r="H13" s="3">
         <v>1</v>
       </c>
       <c r="I13" s="10">
-        <v>0.25490000000000002</v>
+        <v>0.26562999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1397,13 +1397,13 @@
         <v>159</v>
       </c>
       <c r="G14" s="3">
-        <v>0.25490000000000002</v>
+        <v>0.26562999999999998</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
       </c>
       <c r="I14" s="10">
-        <v>0.25490000000000002</v>
+        <v>0.26562999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1426,13 +1426,13 @@
         <v>160</v>
       </c>
       <c r="G15" s="3">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
       <c r="H15" s="3">
         <v>1</v>
       </c>
       <c r="I15" s="10">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1455,13 +1455,13 @@
         <v>160</v>
       </c>
       <c r="G16" s="3">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
       <c r="H16" s="3">
         <v>1</v>
       </c>
       <c r="I16" s="10">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1484,13 +1484,13 @@
         <v>161</v>
       </c>
       <c r="G17" s="3">
-        <v>0.34881000000000001</v>
+        <v>0.36349999999999999</v>
       </c>
       <c r="H17" s="3">
         <v>1</v>
       </c>
       <c r="I17" s="10">
-        <v>0.34881000000000001</v>
+        <v>0.36349999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1538,13 +1538,13 @@
         <v>163</v>
       </c>
       <c r="G19" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H19" s="3">
         <v>1</v>
       </c>
       <c r="I19" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1567,42 +1567,42 @@
         <v>163</v>
       </c>
       <c r="G20" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H20" s="3">
         <v>1</v>
       </c>
       <c r="I20" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>156</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G21" s="3">
-        <v>0.44272</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H21" s="3">
         <v>1</v>
       </c>
       <c r="I21" s="10">
-        <v>0.44272</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1625,13 +1625,13 @@
         <v>163</v>
       </c>
       <c r="G22" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H22" s="3">
         <v>1</v>
       </c>
       <c r="I22" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1654,13 +1654,13 @@
         <v>164</v>
       </c>
       <c r="G23" s="3">
-        <v>0.44272</v>
+        <v>0.46135999999999999</v>
       </c>
       <c r="H23" s="3">
         <v>1</v>
       </c>
       <c r="I23" s="10">
-        <v>0.44272</v>
+        <v>0.46135999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1683,13 +1683,13 @@
         <v>165</v>
       </c>
       <c r="G24" s="3">
-        <v>0.14757000000000001</v>
+        <v>0.15379000000000001</v>
       </c>
       <c r="H24" s="3">
         <v>1</v>
       </c>
       <c r="I24" s="10">
-        <v>0.14757000000000001</v>
+        <v>0.15379000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1712,13 +1712,13 @@
         <v>160</v>
       </c>
       <c r="G25" s="3">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
       <c r="H25" s="3">
         <v>1</v>
       </c>
       <c r="I25" s="10">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1741,13 +1741,13 @@
         <v>163</v>
       </c>
       <c r="G26" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H26" s="3">
         <v>1</v>
       </c>
       <c r="I26" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1795,13 +1795,13 @@
         <v>160</v>
       </c>
       <c r="G28" s="3">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
       <c r="H28" s="3">
         <v>1</v>
       </c>
       <c r="I28" s="10">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1824,13 +1824,13 @@
         <v>163</v>
       </c>
       <c r="G29" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H29" s="3">
         <v>1</v>
       </c>
       <c r="I29" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1878,13 +1878,13 @@
         <v>160</v>
       </c>
       <c r="G31" s="3">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
       <c r="H31" s="3">
         <v>1</v>
       </c>
       <c r="I31" s="10">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1907,13 +1907,13 @@
         <v>164</v>
       </c>
       <c r="G32" s="3">
-        <v>0.44272</v>
+        <v>0.46135999999999999</v>
       </c>
       <c r="H32" s="3">
         <v>1</v>
       </c>
       <c r="I32" s="10">
-        <v>0.44272</v>
+        <v>0.46135999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1936,13 +1936,13 @@
         <v>160</v>
       </c>
       <c r="G33" s="3">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
       <c r="H33" s="3">
         <v>1</v>
       </c>
       <c r="I33" s="10">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1965,13 +1965,13 @@
         <v>160</v>
       </c>
       <c r="G34" s="3">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
       <c r="H34" s="3">
         <v>1</v>
       </c>
       <c r="I34" s="10">
-        <v>0.33539999999999998</v>
+        <v>0.34950999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1994,13 +1994,13 @@
         <v>166</v>
       </c>
       <c r="G35" s="3">
-        <v>1.72</v>
+        <v>1.79</v>
       </c>
       <c r="H35" s="3">
         <v>1</v>
       </c>
       <c r="I35" s="10">
-        <v>1.72</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2023,13 +2023,13 @@
         <v>167</v>
       </c>
       <c r="G36" s="3">
-        <v>0.80495000000000005</v>
+        <v>0.83884000000000003</v>
       </c>
       <c r="H36" s="3">
         <v>1</v>
       </c>
       <c r="I36" s="10">
-        <v>0.80495000000000005</v>
+        <v>0.83884000000000003</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2052,13 +2052,13 @@
         <v>168</v>
       </c>
       <c r="G37" s="3">
-        <v>0.59030000000000005</v>
+        <v>0.61514999999999997</v>
       </c>
       <c r="H37" s="3">
         <v>1</v>
       </c>
       <c r="I37" s="10">
-        <v>0.59030000000000005</v>
+        <v>0.61514999999999997</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2081,13 +2081,13 @@
         <v>169</v>
       </c>
       <c r="G38" s="3">
-        <v>0.18781999999999999</v>
+        <v>0.19572999999999999</v>
       </c>
       <c r="H38" s="3">
         <v>1</v>
       </c>
       <c r="I38" s="10">
-        <v>0.18781999999999999</v>
+        <v>0.19572999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2110,13 +2110,13 @@
         <v>170</v>
       </c>
       <c r="G39" s="3">
-        <v>0.18781999999999999</v>
+        <v>0.19572999999999999</v>
       </c>
       <c r="H39" s="3">
         <v>1</v>
       </c>
       <c r="I39" s="10">
-        <v>0.18781999999999999</v>
+        <v>0.19572999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2139,13 +2139,13 @@
         <v>171</v>
       </c>
       <c r="G40" s="3">
-        <v>20.149999999999999</v>
+        <v>19.989999999999998</v>
       </c>
       <c r="H40" s="3">
         <v>1</v>
       </c>
       <c r="I40" s="10">
-        <v>20.149999999999999</v>
+        <v>19.989999999999998</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2168,13 +2168,13 @@
         <v>172</v>
       </c>
       <c r="G41" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H41" s="3">
         <v>1</v>
       </c>
       <c r="I41" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2197,13 +2197,13 @@
         <v>173</v>
       </c>
       <c r="G42" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H42" s="3">
         <v>1</v>
       </c>
       <c r="I42" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2226,13 +2226,13 @@
         <v>174</v>
       </c>
       <c r="G43" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H43" s="3">
         <v>1</v>
       </c>
       <c r="I43" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2255,13 +2255,13 @@
         <v>174</v>
       </c>
       <c r="G44" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H44" s="3">
         <v>1</v>
       </c>
       <c r="I44" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2284,13 +2284,13 @@
         <v>175</v>
       </c>
       <c r="G45" s="3">
-        <v>0.46955999999999998</v>
+        <v>0.48931999999999998</v>
       </c>
       <c r="H45" s="3">
         <v>1</v>
       </c>
       <c r="I45" s="10">
-        <v>0.46955999999999998</v>
+        <v>0.48931999999999998</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2313,13 +2313,13 @@
         <v>175</v>
       </c>
       <c r="G46" s="3">
-        <v>0.46955999999999998</v>
+        <v>0.48931999999999998</v>
       </c>
       <c r="H46" s="3">
         <v>1</v>
       </c>
       <c r="I46" s="10">
-        <v>0.46955999999999998</v>
+        <v>0.48931999999999998</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2342,13 +2342,13 @@
         <v>176</v>
       </c>
       <c r="G47" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H47" s="3">
         <v>1</v>
       </c>
       <c r="I47" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2371,13 +2371,13 @@
         <v>177</v>
       </c>
       <c r="G48" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H48" s="3">
         <v>1</v>
       </c>
       <c r="I48" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2400,13 +2400,13 @@
         <v>174</v>
       </c>
       <c r="G49" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H49" s="3">
         <v>1</v>
       </c>
       <c r="I49" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2429,13 +2429,13 @@
         <v>178</v>
       </c>
       <c r="G50" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H50" s="3">
         <v>1</v>
       </c>
       <c r="I50" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2458,13 +2458,13 @@
         <v>178</v>
       </c>
       <c r="G51" s="3">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
       <c r="H51" s="3">
         <v>1</v>
       </c>
       <c r="I51" s="10">
-        <v>0.13416</v>
+        <v>0.13980999999999999</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2487,13 +2487,13 @@
         <v>179</v>
       </c>
       <c r="G52" s="3">
-        <v>0.87202999999999997</v>
+        <v>0.88078000000000001</v>
       </c>
       <c r="H52" s="3">
         <v>1</v>
       </c>
       <c r="I52" s="10">
-        <v>0.87202999999999997</v>
+        <v>0.88078000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2516,13 +2516,13 @@
         <v>180</v>
       </c>
       <c r="G53" s="3">
-        <v>5.7</v>
+        <v>5.94</v>
       </c>
       <c r="H53" s="3">
         <v>1</v>
       </c>
       <c r="I53" s="10">
-        <v>5.7</v>
+        <v>5.94</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2545,13 +2545,13 @@
         <v>181</v>
       </c>
       <c r="G54" s="3">
-        <v>3.56</v>
+        <v>3.89</v>
       </c>
       <c r="H54" s="3">
         <v>1</v>
       </c>
       <c r="I54" s="10">
-        <v>3.56</v>
+        <v>3.89</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2574,13 +2574,13 @@
         <v>182</v>
       </c>
       <c r="G55" s="3">
-        <v>2.87</v>
+        <v>2.91</v>
       </c>
       <c r="H55" s="3">
         <v>1</v>
       </c>
       <c r="I55" s="10">
-        <v>2.87</v>
+        <v>2.91</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
@@ -2603,13 +2603,13 @@
         <v>183</v>
       </c>
       <c r="G56" s="3">
-        <v>8.34</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="H56" s="3">
         <v>1</v>
       </c>
       <c r="I56" s="10">
-        <v>8.34</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2632,13 +2632,13 @@
         <v>184</v>
       </c>
       <c r="G57" s="3">
-        <v>16.88</v>
+        <v>17.07</v>
       </c>
       <c r="H57" s="3">
         <v>1</v>
       </c>
       <c r="I57" s="10">
-        <v>16.88</v>
+        <v>17.07</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2661,13 +2661,13 @@
         <v>166</v>
       </c>
       <c r="G58" s="3">
-        <v>1.72</v>
+        <v>1.79</v>
       </c>
       <c r="H58" s="3">
         <v>1</v>
       </c>
       <c r="I58" s="10">
-        <v>1.72</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2690,13 +2690,13 @@
         <v>185</v>
       </c>
       <c r="G59" s="3">
-        <v>5.14</v>
+        <v>5.35</v>
       </c>
       <c r="H59" s="3">
         <v>1</v>
       </c>
       <c r="I59" s="10">
-        <v>5.14</v>
+        <v>5.35</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -2712,7 +2712,7 @@
       </c>
       <c r="I60" s="14">
         <f>SUM(I12:I59)</f>
-        <v>76.812720000000013</v>
+        <v>78.265010000000004</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -2746,7 +2746,7 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="60" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup scale="58" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;BAltium Limited Confidential&amp;B&amp;C&amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
@@ -2888,7 +2888,7 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="97" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="93" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>